<commit_message>
Initial commit - Code update II
</commit_message>
<xml_diff>
--- a/src/test/java/qa/testData/testdata.xlsx
+++ b/src/test/java/qa/testData/testdata.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/freshworks/IdeaProjects/DemoProject/src/test/java/qa/testData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{696696D0-A7A0-594F-A674-756B45F308D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16B61BEA-704E-A94B-8907-09EECEC0D30F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7880" yWindow="4060" windowWidth="14000" windowHeight="10020" xr2:uid="{0B570509-04E2-C742-9AB0-AF7C15DD5FE4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Demo" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,12 +36,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Search Text</t>
   </si>
   <si>
     <t>Active Sync</t>
+  </si>
+  <si>
+    <t>Cat</t>
+  </si>
+  <si>
+    <t>Active Sync2</t>
   </si>
 </sst>
 </file>
@@ -402,9 +408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8F0280E-FE78-6A43-B9E3-28CB1588CEC7}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -418,6 +426,16 @@
         <v>1</v>
       </c>
     </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>